<commit_message>
All set for studying...
</commit_message>
<xml_diff>
--- a/TestEngine/www/testmats/ANSWERS.xlsx
+++ b/TestEngine/www/testmats/ANSWERS.xlsx
@@ -69,14 +69,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,10 +373,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:B86"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A12" sqref="A12:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -474,159 +468,6 @@
       <c r="B11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
-    </row>
-    <row r="22" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-    </row>
-    <row r="27" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="1"/>
-    </row>
-    <row r="31" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="1"/>
-    </row>
-    <row r="32" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="1"/>
-    </row>
-    <row r="34" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="1"/>
-    </row>
-    <row r="35" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="1"/>
-    </row>
-    <row r="36" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="1"/>
-    </row>
-    <row r="37" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="1"/>
-    </row>
-    <row r="38" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="1"/>
-    </row>
-    <row r="39" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="1"/>
-    </row>
-    <row r="40" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="1"/>
-    </row>
-    <row r="41" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="1"/>
-    </row>
-    <row r="42" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="1"/>
-    </row>
-    <row r="43" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="1"/>
-    </row>
-    <row r="44" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="1"/>
-    </row>
-    <row r="46" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="1"/>
-    </row>
-    <row r="47" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="1"/>
-    </row>
-    <row r="48" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="1"/>
-    </row>
-    <row r="49" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="1"/>
-    </row>
-    <row r="50" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="1"/>
-    </row>
-    <row r="53" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="1"/>
-    </row>
-    <row r="54" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="1"/>
-    </row>
-    <row r="55" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="1"/>
-    </row>
-    <row r="56" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="1"/>
-    </row>
-    <row r="57" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="1"/>
-    </row>
-    <row r="58" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="1"/>
-    </row>
-    <row r="59" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="1"/>
-    </row>
-    <row r="60" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="2"/>
-    </row>
-    <row r="62" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="1"/>
-    </row>
-    <row r="63" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="1"/>
-    </row>
-    <row r="64" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="1"/>
-    </row>
-    <row r="65" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="1"/>
-    </row>
-    <row r="66" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="1"/>
-    </row>
-    <row r="68" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="1"/>
-    </row>
-    <row r="69" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="1"/>
-    </row>
-    <row r="70" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="1"/>
-    </row>
-    <row r="71" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="1"/>
-    </row>
-    <row r="72" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="1"/>
-    </row>
-    <row r="73" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="1"/>
-    </row>
-    <row r="74" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="1"/>
-    </row>
-    <row r="75" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="1"/>
-    </row>
-    <row r="77" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="1"/>
-    </row>
-    <row r="78" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="1"/>
-    </row>
-    <row r="79" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="1"/>
-    </row>
-    <row r="81" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="1"/>
-    </row>
-    <row r="82" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="1"/>
-    </row>
-    <row r="83" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="1"/>
-    </row>
-    <row r="84" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="1"/>
-    </row>
-    <row r="85" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="1"/>
-    </row>
-    <row r="86" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added more..had an improvement idea..commented
</commit_message>
<xml_diff>
--- a/TestEngine/www/testmats/ANSWERS.xlsx
+++ b/TestEngine/www/testmats/ANSWERS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="6">
   <si>
     <t>ANSWER</t>
   </si>
@@ -69,8 +69,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -373,10 +380,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:F209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD1048576"/>
+      <selection activeCell="C209" sqref="C209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -467,6 +474,1800 @@
       </c>
       <c r="B11" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+    </row>
+    <row r="35" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+    </row>
+    <row r="36" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+    </row>
+    <row r="37" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+    </row>
+    <row r="38" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+    </row>
+    <row r="39" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+    </row>
+    <row r="40" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+    </row>
+    <row r="41" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+    </row>
+    <row r="43" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+    </row>
+    <row r="44" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+    </row>
+    <row r="45" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+    </row>
+    <row r="47" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+    </row>
+    <row r="48" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+    </row>
+    <row r="49" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+    </row>
+    <row r="50" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+    </row>
+    <row r="51" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C51" s="1"/>
+    </row>
+    <row r="52" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" s="1"/>
+    </row>
+    <row r="53" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+    </row>
+    <row r="54" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+    </row>
+    <row r="55" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+    </row>
+    <row r="56" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+    </row>
+    <row r="57" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+    </row>
+    <row r="58" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+    </row>
+    <row r="59" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+    </row>
+    <row r="60" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C60" s="2"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+    </row>
+    <row r="61" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+    </row>
+    <row r="62" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+    </row>
+    <row r="63" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+    </row>
+    <row r="64" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+    </row>
+    <row r="65" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+    </row>
+    <row r="66" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+    </row>
+    <row r="67" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+    </row>
+    <row r="68" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+    </row>
+    <row r="69" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+    </row>
+    <row r="70" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+    </row>
+    <row r="71" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+    </row>
+    <row r="72" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+    </row>
+    <row r="73" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+    </row>
+    <row r="74" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+    </row>
+    <row r="75" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+    </row>
+    <row r="76" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C76" s="1"/>
+    </row>
+    <row r="77" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+    </row>
+    <row r="78" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+    </row>
+    <row r="79" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1"/>
+    </row>
+    <row r="80" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F80" s="1"/>
+    </row>
+    <row r="81" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
+    </row>
+    <row r="82" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="F82" s="1"/>
+    </row>
+    <row r="83" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+      <c r="F83" s="1"/>
+    </row>
+    <row r="84" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+      <c r="F84" s="1"/>
+    </row>
+    <row r="85" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C85" s="1"/>
+      <c r="D85" s="1"/>
+      <c r="E85" s="1"/>
+      <c r="F85" s="1"/>
+    </row>
+    <row r="86" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1"/>
+    </row>
+    <row r="87" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>105</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>106</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>107</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>108</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>109</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>110</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>111</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>112</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>113</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>114</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>115</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>116</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>117</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>118</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>119</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>120</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>121</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>122</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>123</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>124</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>125</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>126</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>127</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>128</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>129</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>130</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>131</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>132</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>133</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>134</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>135</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>136</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>137</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>138</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>139</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>140</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>141</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>142</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>143</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>144</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>145</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>146</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>147</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>148</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>149</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>150</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>151</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>152</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>153</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>154</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>155</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>156</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>157</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>158</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>159</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>160</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>161</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>162</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>163</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>164</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>165</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>166</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>167</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>168</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>169</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>170</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>171</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>172</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>173</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>174</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>175</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>176</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>177</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>178</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>179</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>180</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>181</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>182</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>183</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>184</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>185</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>186</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>187</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>188</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>189</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>190</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>191</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>192</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>193</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>194</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>195</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>196</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>197</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>198</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>199</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>200</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>201</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>202</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>203</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>204</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>205</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>206</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>207</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>208</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Randomized questions instead of subsetting chunks of questions
</commit_message>
<xml_diff>
--- a/TestEngine/www/testmats/ANSWERS.xlsx
+++ b/TestEngine/www/testmats/ANSWERS.xlsx
@@ -69,7 +69,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -77,7 +77,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,10 +379,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F209"/>
+  <dimension ref="A1:B209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C209" sqref="C209"/>
+      <selection activeCell="C1" sqref="C1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -516,19 +515,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -536,7 +531,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -544,7 +539,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -552,7 +547,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -560,19 +555,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -580,7 +571,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -588,7 +579,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -596,7 +587,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -604,19 +595,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -624,7 +611,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -632,7 +619,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -640,31 +627,23 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -672,138 +651,95 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-    </row>
-    <row r="35" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-    </row>
-    <row r="36" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-    </row>
-    <row r="37" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-    </row>
-    <row r="38" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-    </row>
-    <row r="39" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-    </row>
-    <row r="40" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-    </row>
-    <row r="41" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-    </row>
-    <row r="42" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-    </row>
-    <row r="43" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-    </row>
-    <row r="44" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-    </row>
-    <row r="45" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -811,482 +747,335 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-    </row>
-    <row r="47" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-    </row>
-    <row r="48" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-    </row>
-    <row r="49" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-    </row>
-    <row r="50" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-    </row>
-    <row r="51" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C51" s="1"/>
-    </row>
-    <row r="52" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C52" s="1"/>
-    </row>
-    <row r="53" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-    </row>
-    <row r="54" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-    </row>
-    <row r="55" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-    </row>
-    <row r="56" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-    </row>
-    <row r="57" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
-    </row>
-    <row r="58" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
-    </row>
-    <row r="59" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
-    </row>
-    <row r="60" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C60" s="2"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
-    </row>
-    <row r="61" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
-    </row>
-    <row r="62" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
-    </row>
-    <row r="63" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
-    </row>
-    <row r="64" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
-    </row>
-    <row r="65" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
-    </row>
-    <row r="66" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
-      <c r="F66" s="1"/>
-    </row>
-    <row r="67" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E67" s="1"/>
-      <c r="F67" s="1"/>
-    </row>
-    <row r="68" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
-      <c r="F68" s="1"/>
-    </row>
-    <row r="69" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
-    </row>
-    <row r="70" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
-    </row>
-    <row r="71" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
-    </row>
-    <row r="72" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
-    </row>
-    <row r="73" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
-    </row>
-    <row r="74" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
-    </row>
-    <row r="75" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C75" s="1"/>
-      <c r="D75" s="1"/>
-      <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
-    </row>
-    <row r="76" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C76" s="1"/>
-    </row>
-    <row r="77" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C77" s="1"/>
-      <c r="D77" s="1"/>
-      <c r="E77" s="1"/>
-      <c r="F77" s="1"/>
-    </row>
-    <row r="78" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C78" s="1"/>
-      <c r="D78" s="1"/>
-      <c r="E78" s="1"/>
-      <c r="F78" s="1"/>
-    </row>
-    <row r="79" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C79" s="1"/>
-      <c r="D79" s="1"/>
-      <c r="E79" s="1"/>
-      <c r="F79" s="1"/>
-    </row>
-    <row r="80" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F80" s="1"/>
-    </row>
-    <row r="81" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C81" s="1"/>
-      <c r="D81" s="1"/>
-      <c r="E81" s="1"/>
-      <c r="F81" s="1"/>
-    </row>
-    <row r="82" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C82" s="1"/>
-      <c r="D82" s="1"/>
-      <c r="E82" s="1"/>
-      <c r="F82" s="1"/>
-    </row>
-    <row r="83" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
-      <c r="E83" s="1"/>
-      <c r="F83" s="1"/>
-    </row>
-    <row r="84" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C84" s="1"/>
-      <c r="D84" s="1"/>
-      <c r="E84" s="1"/>
-      <c r="F84" s="1"/>
-    </row>
-    <row r="85" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C85" s="1"/>
-      <c r="D85" s="1"/>
-      <c r="E85" s="1"/>
-      <c r="F85" s="1"/>
-    </row>
-    <row r="86" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C86" s="1"/>
-      <c r="D86" s="1"/>
-      <c r="E86" s="1"/>
-      <c r="F86" s="1"/>
-    </row>
-    <row r="87" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -1294,7 +1083,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -1302,7 +1091,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -1310,7 +1099,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -1318,7 +1107,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -1326,7 +1115,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -1334,7 +1123,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -1342,7 +1131,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -1350,7 +1139,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -1358,7 +1147,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>

</xml_diff>